<commit_message>
tried to preload realm data
</commit_message>
<xml_diff>
--- a/chatter_topics.xlsx
+++ b/chatter_topics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sy/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sy/Desktop/Chatter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF21D21-DC97-CB42-9981-9A20DDBBDB1D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E84BD7-79E1-B441-A486-0FA6B8403FBB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="460" windowWidth="22220" windowHeight="14660" activeTab="4" xr2:uid="{B1BB7CA4-FF86-6747-B354-6715F01FF785}"/>
+    <workbookView xWindow="4720" yWindow="460" windowWidth="22220" windowHeight="13080" activeTab="4" xr2:uid="{B1BB7CA4-FF86-6747-B354-6715F01FF785}"/>
   </bookViews>
   <sheets>
     <sheet name="Good for all" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="132">
   <si>
     <t>Set I</t>
   </si>
@@ -91,406 +91,434 @@
     <t>Got any fun plans for the weekend? I need some inspiration so I don't end up on the couch with some Netflix and Ben &amp; Jerry's.</t>
   </si>
   <si>
+    <t>On what topic do people always come to you with questions?</t>
+  </si>
+  <si>
+    <t>Who was your childhood hero?</t>
+  </si>
+  <si>
+    <t>Do you have a secret talent?</t>
+  </si>
+  <si>
+    <t>Working on anything exciting lately?</t>
+  </si>
+  <si>
+    <t>What was the highlight of your week?</t>
+  </si>
+  <si>
+    <t>What is something you are obsessed with?</t>
+  </si>
+  <si>
+    <t>Who is your favorite entertainer (comedian, musician, actor, etc.)?</t>
+  </si>
+  <si>
+    <t>What’s the best / worst thing about your work?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What three words best describe you?</t>
+  </si>
+  <si>
+    <t>What would be your perfect weekend?</t>
+  </si>
+  <si>
+    <t>What is your guilty pleasure?</t>
+  </si>
+  <si>
+    <t>What was the best time period of your life?</t>
+  </si>
+  <si>
+    <t>What would be the most amazing adventure to go on?</t>
+  </si>
+  <si>
+    <t>When are you happiest?</t>
+  </si>
+  <si>
+    <t>What’s the most interesting fact you know?</t>
+  </si>
+  <si>
+    <t>What’s The Weirdest Gift You Ever Received?</t>
+  </si>
+  <si>
+    <t>If you could live your life again knowing what you do now, what would you change?</t>
+  </si>
+  <si>
+    <t>What do you love about your job?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>How did you get into the industry?</t>
+  </si>
+  <si>
+    <t>What was the last good movie you saw?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is a good book you last read?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>How are things going?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Given the choice of anyone in the world, whom would you want as a dinner guest?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Would you like to be famous? In what way?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Before making a telephone call, do you ever rehearse what you are going to say? Why?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What would constitute a “perfect” day for you?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>When did you last sing to yourself? To someone else?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If you were able to live to the age of 90 and retain either the mind or body of a 30-year-old for the last 60 years of your life, which would you want?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Do you have a secret hunch about how you will die?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name three things you and your partner appear to have in common.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For what in your life do you feel most grateful?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If you could change anything about the way you were raised, what would it be?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Take four minutes and tell your partner your life story in as much detail as possible.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If you could wake up tomorrow having gained any one quality or ability, what would it be?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If a crystal ball could tell you the truth about yourself, your life, the future or anything else, what would you want to know?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is there something that you’ve dreamed of doing for a long time? Why haven’t you done it?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is the greatest accomplishment of your life?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What do you value most in a friendship?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is your most treasured memory?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is your most terrible memory?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If you knew that in one year you would die suddenly, would you change anything about the way you are now living? Why?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What does friendship mean to you?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What roles do love and affection play in your life?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alternate sharing something you consider a positive characteristic of your partner. Share a total of five items.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>How close and warm is your family? Do you feel your childhood was happier than most other people’s?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>How do you feel about your relationship with your mother?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Make three true “we” statements each. For instance, “We are both in this room feeling ... “</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete this sentence: “I wish I had someone with whom I could share ... “</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If you were going to become a close friend with your partner, please share what would be important for him or her to know.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tell your partner what you like about them; be very honest this time, saying things that you might not say to someone you’ve just met.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Share with your partner an embarrassing moment in your life.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>When did you last cry in front of another person? By yourself?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tell your partner something that you like about them already.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What, if anything, is too serious to be joked about?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If you were to die this evening with no opportunity to communicate with anyone, what would you most regret not having told someone? Why haven’t you told them yet?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Your house, containing everything you own, catches fire. After saving your loved ones and pets, you have time to safely make a final dash to save any one item. What would it be? Why?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Of all the people in your family, whose death would you find most disturbing? Why?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Share a personal problem and ask your partner’s advice on how he or she might handle it. Also, ask your partner to reflect back to you how you seem to be feeling about the problem you have chosen.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What was the best piece of advice you got early on in your career?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What’s the most exciting thing about your industry?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What’s your biggest priority right now?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What’s your progress on [X goal]?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>As an expert in [field], I’d love to hear your thoughts on [event, announcement, major change].</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is a typical day like for you?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What do you hope to get out of today?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What's your favorite part about living in [city]? Least favorite?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Why did you come tonight?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is your day going like you expected?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What’s your story?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What was the highlight of your week?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Which season are you most active in?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What do you like to do in spring?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is your favorite holiday?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Where is the most interesting place you’ve been?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What was the best time period of your life?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What was the best book or series that you’ve ever read?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What are you passionate about?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What was the last photo you took?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Are you looking forward to anything in the next few weeks?</t>
-  </si>
-  <si>
-    <t>On what topic do people always come to you with questions?</t>
-  </si>
-  <si>
-    <t>Who was your childhood hero?</t>
-  </si>
-  <si>
-    <t>Do you have a secret talent?</t>
-  </si>
-  <si>
-    <t>Working on anything exciting lately?</t>
-  </si>
-  <si>
-    <t>What was the highlight of your week?</t>
-  </si>
-  <si>
-    <t>What is something you are obsessed with?</t>
-  </si>
-  <si>
-    <t>Who is your favorite entertainer (comedian, musician, actor, etc.)?</t>
-  </si>
-  <si>
-    <t>What’s the best / worst thing about your work?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What three words best describe you?</t>
-  </si>
-  <si>
-    <t>What would be your perfect weekend?</t>
-  </si>
-  <si>
-    <t>What is your guilty pleasure?</t>
-  </si>
-  <si>
-    <t>What was the best time period of your life?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What’s the best thing that happened to you last week?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What one thing do you really want but can’t afford?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is special about the place you grew up?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anything exciting going on this week?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What are some of the best vacations you’ve had?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What’s the most interesting thing you’ve read or seen this week?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What’s the most amazing true story you’ve heard?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What’s keeping you busy lately?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is the best piece of advice you've received?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What's your favorite part of the event so far?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What are the best opportunities that you see ahead of you this year?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What do you do to improve your mood when you are in a bad mood?</t>
-  </si>
-  <si>
-    <t>What are some things you want to accomplish before you die?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What are some things you want to accomplish?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What are you best at?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What is the craziest, most outrageous thing you want to achieve?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>How have your goals changed over your life?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>How much do you plan for the future?</t>
-  </si>
-  <si>
-    <t>What would be the most amazing adventure to go on?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What are some small things that make your day better?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What is the most heartwarming thing you’ve ever seen?</t>
-  </si>
-  <si>
-    <t>Where is the most interesting place you’ve been?</t>
-  </si>
-  <si>
-    <t>What’s the best thing that happened to you last week?</t>
-  </si>
-  <si>
-    <t>What one thing do you really want but can’t afford?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Where do you usually go when you when you have time off?</t>
-  </si>
-  <si>
-    <t>What is special about the place you grew up?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What were some of the turning points in your life?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What do you spend the most time thinking about?</t>
-  </si>
-  <si>
-    <t>What were some of the turning points in your life?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What are three interesting facts about you?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What stresses you out the most?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What problem are you currently grappling with?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What’s the title of the current chapter of your life?</t>
-  </si>
-  <si>
-    <t>What was the last photo you took?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What did you Google last?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What food do you crave most often?</t>
-  </si>
-  <si>
-    <t>Anything exciting going on this week?</t>
-  </si>
-  <si>
-    <t>What stresses you out the most?</t>
-  </si>
-  <si>
-    <t>When are you happiest?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Do you have any brands that you are really loyal to?</t>
-  </si>
-  <si>
-    <t>What’s the most interesting fact you know?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>If You Could Have Dinner With Any, Currently Alive, Person In The World, Who Would It Be?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>If You Could Be Anywhere Now, Where Would You Be?</t>
-  </si>
-  <si>
-    <t>What’s The Weirdest Gift You Ever Received?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What is the best and worst purchases you’ve ever made?</t>
-  </si>
-  <si>
-    <t>What’s the most interesting thing you’ve read or seen this week?</t>
-  </si>
-  <si>
-    <t>If you could live your life again knowing what you do now, what would you change?</t>
-  </si>
-  <si>
-    <t>What problem are you currently grappling with?</t>
-  </si>
-  <si>
-    <t>What are some of the best vacations you’ve had?</t>
-  </si>
-  <si>
-    <t>What’s the most amazing true story you’ve heard?</t>
-  </si>
-  <si>
-    <t>What do you love about your job?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What's your favorite part of the event so far?</t>
-  </si>
-  <si>
-    <t>How did you get into the industry?</t>
-  </si>
-  <si>
-    <t>What was the last good movie you saw?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is a good book you last read?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What’s keeping you busy lately?</t>
-  </si>
-  <si>
-    <t>What are the best opportunities that you see ahead of you this year?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What was the last thing you purchased?</t>
-  </si>
-  <si>
-    <t>What is the best piece of advice you've received?</t>
-  </si>
-  <si>
-    <t>How are things going?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Given the choice of anyone in the world, whom would you want as a dinner guest?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Would you like to be famous? In what way?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Before making a telephone call, do you ever rehearse what you are going to say? Why?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What would constitute a “perfect” day for you?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>When did you last sing to yourself? To someone else?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If you were able to live to the age of 90 and retain either the mind or body of a 30-year-old for the last 60 years of your life, which would you want?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Do you have a secret hunch about how you will die?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name three things you and your partner appear to have in common.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>For what in your life do you feel most grateful?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If you could change anything about the way you were raised, what would it be?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Take four minutes and tell your partner your life story in as much detail as possible.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If you could wake up tomorrow having gained any one quality or ability, what would it be?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If a crystal ball could tell you the truth about yourself, your life, the future or anything else, what would you want to know?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Is there something that you’ve dreamed of doing for a long time? Why haven’t you done it?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is the greatest accomplishment of your life?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What do you value most in a friendship?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is your most treasured memory?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is your most terrible memory?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If you knew that in one year you would die suddenly, would you change anything about the way you are now living? Why?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What does friendship mean to you?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What roles do love and affection play in your life?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Alternate sharing something you consider a positive characteristic of your partner. Share a total of five items.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>How close and warm is your family? Do you feel your childhood was happier than most other people’s?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>How do you feel about your relationship with your mother?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Make three true “we” statements each. For instance, “We are both in this room feeling ... “</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete this sentence: “I wish I had someone with whom I could share ... “</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If you were going to become a close friend with your partner, please share what would be important for him or her to know.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tell your partner what you like about them; be very honest this time, saying things that you might not say to someone you’ve just met.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Share with your partner an embarrassing moment in your life.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>When did you last cry in front of another person? By yourself?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tell your partner something that you like about them already.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What, if anything, is too serious to be joked about?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If you were to die this evening with no opportunity to communicate with anyone, what would you most regret not having told someone? Why haven’t you told them yet?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Your house, containing everything you own, catches fire. After saving your loved ones and pets, you have time to safely make a final dash to save any one item. What would it be? Why?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Of all the people in your family, whose death would you find most disturbing? Why?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Share a personal problem and ask your partner’s advice on how he or she might handle it. Also, ask your partner to reflect back to you how you seem to be feeling about the problem you have chosen.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What was the best piece of advice you got early on in your career?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What’s the most exciting thing about your industry?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What’s your biggest priority right now?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What’s your progress on [X goal]?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>As an expert in [field], I’d love to hear your thoughts on [event, announcement, major change].</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is a typical day like for you?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What do you hope to get out of today?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What's your favorite part about living in [city]? Least favorite?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Why did you come tonight?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Is your day going like you expected?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What’s your story?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What was the highlight of your week?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Which season are you most active in?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What do you like to do in spring?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is your favorite holiday?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Where is the most interesting place you’ve been?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What was the best time period of your life?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What was the best book or series that you’ve ever read?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What are you passionate about?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>What was the last photo you took?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -595,12 +623,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -617,7 +651,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -661,6 +695,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -979,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5628426C-42F1-5A49-8AA8-44D26D2E2A58}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -992,7 +1047,7 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3"/>
@@ -1002,7 +1057,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1011,7 +1066,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1019,8 +1074,8 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="4" t="s">
-        <v>123</v>
+      <c r="A5" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1029,7 +1084,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1037,8 +1092,8 @@
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="6" t="s">
-        <v>124</v>
+      <c r="A7" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1046,8 +1101,8 @@
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
-        <v>125</v>
+      <c r="A8" s="16" t="s">
+        <v>89</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1056,7 +1111,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1065,7 +1120,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1073,8 +1128,8 @@
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="5" t="s">
-        <v>127</v>
+      <c r="A11" s="17" t="s">
+        <v>91</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1082,8 +1137,8 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="5" t="s">
-        <v>128</v>
+      <c r="A12" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1091,8 +1146,8 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="5" t="s">
-        <v>131</v>
+      <c r="A13" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1100,8 +1155,8 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="5" t="s">
-        <v>129</v>
+      <c r="A14" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1109,8 +1164,8 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="5" t="s">
-        <v>43</v>
+      <c r="A15" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1118,8 +1173,8 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="5" t="s">
-        <v>44</v>
+      <c r="A16" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1127,8 +1182,8 @@
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="5" t="s">
-        <v>46</v>
+      <c r="A17" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1136,8 +1191,8 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="5" t="s">
-        <v>133</v>
+      <c r="A18" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1145,8 +1200,8 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="5" t="s">
-        <v>54</v>
+      <c r="A19" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1154,8 +1209,8 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="5" t="s">
-        <v>63</v>
+      <c r="A20" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1163,8 +1218,8 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="5" t="s">
-        <v>66</v>
+      <c r="A21" s="17" t="s">
+        <v>103</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1172,8 +1227,8 @@
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="5" t="s">
-        <v>67</v>
+      <c r="A22" s="17" t="s">
+        <v>105</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1181,8 +1236,8 @@
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="4" t="s">
-        <v>77</v>
+      <c r="A23" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1190,8 +1245,8 @@
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="5" t="s">
-        <v>71</v>
+      <c r="A24" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1199,8 +1254,8 @@
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="8" t="s">
-        <v>73</v>
+      <c r="A25" s="18" t="s">
+        <v>106</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1208,8 +1263,8 @@
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="6" t="s">
-        <v>76</v>
+      <c r="A26" s="16" t="s">
+        <v>107</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1226,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAB80A1-C584-D044-B8FE-394496A86437}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1238,8 +1293,8 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="9" t="s">
-        <v>78</v>
+      <c r="A3" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1252,8 +1307,8 @@
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="9" t="s">
-        <v>79</v>
+      <c r="A5" s="19" t="s">
+        <v>43</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1267,7 +1322,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="9" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1280,8 +1335,8 @@
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="9" t="s">
-        <v>81</v>
+      <c r="A9" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1294,8 +1349,8 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="9" t="s">
-        <v>82</v>
+      <c r="A11" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1308,8 +1363,8 @@
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="9" t="s">
-        <v>83</v>
+      <c r="A13" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1323,7 +1378,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="9" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1336,8 +1391,8 @@
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="9" t="s">
-        <v>85</v>
+      <c r="A17" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1350,8 +1405,8 @@
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="9" t="s">
-        <v>86</v>
+      <c r="A19" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1364,8 +1419,8 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="9" t="s">
-        <v>87</v>
+      <c r="A21" s="19" t="s">
+        <v>51</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1379,7 +1434,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="9" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1392,8 +1447,8 @@
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="9" t="s">
-        <v>89</v>
+      <c r="A25" s="19" t="s">
+        <v>53</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1421,7 +1476,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="9" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1435,7 +1490,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="9" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1449,7 +1504,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="9" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1463,7 +1518,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="9" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1477,7 +1532,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="9" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1491,7 +1546,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="9" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1505,7 +1560,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="9" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1519,7 +1574,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="9" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1533,7 +1588,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="9" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1547,7 +1602,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="9" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1561,7 +1616,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="9" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1575,7 +1630,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="9" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1603,7 +1658,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="9" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1617,7 +1672,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="9" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -1631,7 +1686,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="9" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -1645,7 +1700,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="9" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -1659,7 +1714,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="9" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -1673,7 +1728,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="9" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -1687,7 +1742,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="9" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -1701,7 +1756,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="9" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -1715,7 +1770,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="9" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -1729,7 +1784,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="9" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -1743,7 +1798,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="9" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -1757,7 +1812,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="9" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -1773,14 +1828,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DF7C0D-58E2-0546-B7A0-DA521DA7A3A5}">
   <dimension ref="A2:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3"/>
@@ -1792,7 +1847,7 @@
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="3"/>
@@ -1804,7 +1859,7 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3"/>
@@ -1816,7 +1871,7 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3"/>
@@ -1828,7 +1883,7 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3"/>
@@ -1840,8 +1895,8 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="4" t="s">
-        <v>21</v>
+      <c r="A7" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1852,8 +1907,8 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="6" t="s">
-        <v>24</v>
+      <c r="A8" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1864,8 +1919,8 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="5" t="s">
-        <v>28</v>
+      <c r="A9" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1877,7 +1932,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1888,8 +1943,8 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="3" t="s">
-        <v>68</v>
+      <c r="A11" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1901,7 +1956,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="13" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1912,8 +1967,8 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="13" t="s">
-        <v>70</v>
+      <c r="A13" s="21" t="s">
+        <v>38</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1925,7 +1980,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="13" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1937,7 +1992,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1949,7 +2004,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1961,7 +2016,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="4" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1973,7 +2028,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1985,7 +2040,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="4" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1997,7 +2052,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="8" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2009,7 +2064,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2021,7 +2076,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="11" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2033,7 +2088,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="12" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2053,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1239FF-31EA-4F40-9FE2-6F99D4FE6630}">
   <dimension ref="A2:A30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2063,148 +2118,148 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="4" t="s">
-        <v>22</v>
+      <c r="A7" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" s="17" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="5" t="s">
-        <v>35</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="5" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="5" t="s">
-        <v>37</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="5" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="5" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="5" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="5" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="5" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2217,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97333F1-FB09-A941-88F5-C033E7BE65A9}">
   <dimension ref="A2:A28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2227,138 +2282,138 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="6" t="s">
-        <v>25</v>
+      <c r="A13" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="5" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="5" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="5" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
-        <v>52</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
-        <v>57</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="5" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="14" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="14" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="14" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="3" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="6" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>